<commit_message>
added template version to properties
</commit_message>
<xml_diff>
--- a/bulk-upload-templates/hu/e-label_excel_import_hu.xlsx
+++ b/bulk-upload-templates/hu/e-label_excel_import_hu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbauer/workspace/vs_code/misc/e-label.io/bulk-upload-templates/hu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A9C8C1-073C-1947-B1B8-981C52FAA287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5DC50C-A054-434E-BF68-D2C220615070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4940" yWindow="2320" windowWidth="30240" windowHeight="17960" xr2:uid="{42B7CF4C-2976-4744-81A6-4766AD4B0A9A}"/>
   </bookViews>
@@ -19521,6 +19521,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="521892c6-de4d-4693-8930-cf3c65837cb3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="8b51d2f0-ad09-4f56-8484-9cdc12a45078" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x010100C7D3B76224FB794FA31A6F74C3DB4B7D" ma:contentTypeVersion="14" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="c64eb670e7585cd8bd7ba1c49946b64c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="521892c6-de4d-4693-8930-cf3c65837cb3" xmlns:ns3="8b51d2f0-ad09-4f56-8484-9cdc12a45078" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b7d7f181e5149163ac5b28d570d1cbda" ns2:_="" ns3:_="">
     <xsd:import namespace="521892c6-de4d-4693-8930-cf3c65837cb3"/>
@@ -19749,17 +19760,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="521892c6-de4d-4693-8930-cf3c65837cb3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="8b51d2f0-ad09-4f56-8484-9cdc12a45078" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -19770,6 +19770,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7AED586-CF85-4589-9067-6F5DCBF267C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="521892c6-de4d-4693-8930-cf3c65837cb3"/>
+    <ds:schemaRef ds:uri="8b51d2f0-ad09-4f56-8484-9cdc12a45078"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04C9E887-07B4-4C1B-B500-0A8783AD8047}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19788,17 +19799,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7AED586-CF85-4589-9067-6F5DCBF267C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="521892c6-de4d-4693-8930-cf3c65837cb3"/>
-    <ds:schemaRef ds:uri="8b51d2f0-ad09-4f56-8484-9cdc12a45078"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78FB99DB-BC6F-4BBF-A5C6-81EABB4A6C5F}">
   <ds:schemaRefs>

</xml_diff>